<commit_message>
cac file trong bao cao
</commit_message>
<xml_diff>
--- a/đatn-test.xlsx
+++ b/đatn-test.xlsx
@@ -5,17 +5,18 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/a7dacad865ed9993/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\SilverStorePrj\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="8_{15C6832F-11FF-4A52-8D6C-27F847B1198E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DA027AFF-40B2-403F-8FA6-C5A0C89B9ABC}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{209AA20D-7423-4EFF-966F-534644EF057E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="1875" windowWidth="10200" windowHeight="7875" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TC List" sheetId="3" r:id="rId1"/>
-    <sheet name="Login" sheetId="1" r:id="rId2"/>
-    <sheet name="Register" sheetId="2" r:id="rId3"/>
+    <sheet name="Đăng nhập" sheetId="1" r:id="rId2"/>
+    <sheet name="Đăng ký" sheetId="2" r:id="rId3"/>
+    <sheet name="QL Danh mục" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="413" uniqueCount="265">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="489" uniqueCount="300">
   <si>
     <t>ID</t>
   </si>
@@ -128,9 +129,6 @@
   </si>
   <si>
     <t>Truy cập vào màn hình bằng cách click link</t>
-  </si>
-  <si>
-    <t>Truy cập vào màn hình bằng cách paste link</t>
   </si>
   <si>
     <t>Test trường hợp vào màn hình bằng cách click link</t>
@@ -858,12 +856,6 @@
     <t>Pre-Condition</t>
   </si>
   <si>
-    <t>Register</t>
-  </si>
-  <si>
-    <t>Login</t>
-  </si>
-  <si>
     <t>Register-26</t>
   </si>
   <si>
@@ -891,14 +883,135 @@
     <t>Register-02</t>
   </si>
   <si>
-    <t>dvvsd</t>
+    <t xml:space="preserve">Đăng ký </t>
+  </si>
+  <si>
+    <t>Đăng nhập</t>
+  </si>
+  <si>
+    <t>CateMng-01</t>
+  </si>
+  <si>
+    <t>CateMng-02</t>
+  </si>
+  <si>
+    <t>CateMng-03</t>
+  </si>
+  <si>
+    <t>CateMng-04</t>
+  </si>
+  <si>
+    <t>CateMng-05</t>
+  </si>
+  <si>
+    <t>CateMng-06</t>
+  </si>
+  <si>
+    <t>CateMng-07</t>
+  </si>
+  <si>
+    <t>CateMng-08</t>
+  </si>
+  <si>
+    <t>CateMng-09</t>
+  </si>
+  <si>
+    <t>CateMng-10</t>
+  </si>
+  <si>
+    <t>CateMng-11</t>
+  </si>
+  <si>
+    <t>CateMng-12</t>
+  </si>
+  <si>
+    <t>CateMng-13</t>
+  </si>
+  <si>
+    <t>CateMng-14</t>
+  </si>
+  <si>
+    <t>CateMng-15</t>
+  </si>
+  <si>
+    <t>CateMng-16</t>
+  </si>
+  <si>
+    <t>CateMng-17</t>
+  </si>
+  <si>
+    <t>CateMng-18</t>
+  </si>
+  <si>
+    <t>CateMng-19</t>
+  </si>
+  <si>
+    <t>CateMng-20</t>
+  </si>
+  <si>
+    <t>CateMng-21</t>
+  </si>
+  <si>
+    <t>CateMng-22</t>
+  </si>
+  <si>
+    <t>CateMng-23</t>
+  </si>
+  <si>
+    <t>CATEGORY MANAGEMENT</t>
+  </si>
+  <si>
+    <t>Truy cập bằng cách đăng nhập và thực hiện các thao tác trên màn hình.</t>
+  </si>
+  <si>
+    <t>Trường hơp user có quyền truy cập trang Quản lý tài khoản</t>
+  </si>
+  <si>
+    <t>Trường hơp user không có quyền truy cập trang Quản lý tài khoản</t>
+  </si>
+  <si>
+    <t>1. Username: caobac.admin01@gmail.com có quyền truy cập vào hệ thống quản trị
+2. Username có quyền truy cập màn hình quản lý danh mục</t>
+  </si>
+  <si>
+    <t>1. Login vào hệ thống bằng username: caobac.admin01@gmail.com
+password: admin12345
+2. Click "Quản lý danh mục" trên thanh menu admin</t>
+  </si>
+  <si>
+    <t>1. Username: caobac.staff01@gmail.com có quyền truy cập vào hệ thống quản trị
+2. Username không có quyền truy cập màn hình quản lý danh mục</t>
+  </si>
+  <si>
+    <t>username: caobac.staff01@gmail.com
+password: staff01</t>
+  </si>
+  <si>
+    <t>username: caobac.admin01@gmail.com
+password: admin01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Đăng nhập thành công, menu hiển thị Quản lý danh mục
+</t>
+  </si>
+  <si>
+    <t>Đăng nhập thành công, menu không hiển thị Quản lý danh mục</t>
+  </si>
+  <si>
+    <t>Login vào hệ thống bằng tài khoản username: caobac.staff01@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Truy cập bằng cách paste url </t>
+  </si>
+  <si>
+    <t>Truy cập vào màn hình bằng cách paste url</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -961,6 +1074,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -976,7 +1095,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="14">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -1073,102 +1192,12 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="90">
+  <cellXfs count="97">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1302,30 +1331,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -1335,21 +1343,15 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -1359,56 +1361,68 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1416,25 +1430,61 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1442,7 +1492,34 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="9">
+  <dxfs count="12">
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFE7A7A"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="9" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FFFF0000"/>
@@ -1813,222 +1890,220 @@
       <pane xSplit="1" ySplit="8" topLeftCell="B9" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A9" sqref="A9"/>
-      <selection pane="bottomRight" activeCell="D11" sqref="D11"/>
+      <selection pane="bottomRight" activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="51"/>
-    <col min="2" max="2" width="16.42578125" style="51" customWidth="1"/>
-    <col min="3" max="3" width="27.140625" style="51" customWidth="1"/>
-    <col min="4" max="4" width="25.85546875" style="51" customWidth="1"/>
-    <col min="5" max="5" width="20.7109375" style="51" customWidth="1"/>
-    <col min="6" max="6" width="19.7109375" style="51" customWidth="1"/>
-    <col min="7" max="16384" width="9.140625" style="51"/>
+    <col min="1" max="1" width="9.140625" style="45"/>
+    <col min="2" max="2" width="16.42578125" style="45" customWidth="1"/>
+    <col min="3" max="3" width="27.140625" style="45" customWidth="1"/>
+    <col min="4" max="4" width="25.85546875" style="79" customWidth="1"/>
+    <col min="5" max="5" width="20.7109375" style="45" customWidth="1"/>
+    <col min="6" max="6" width="19.7109375" style="45" customWidth="1"/>
+    <col min="7" max="16384" width="9.140625" style="45"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:6" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="D1" s="52" t="s">
+      <c r="D1" s="78" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B3" s="47" t="s">
         <v>244</v>
       </c>
-    </row>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B3" s="54" t="s">
+      <c r="C3" s="52"/>
+      <c r="D3" s="53"/>
+      <c r="E3" s="53"/>
+      <c r="F3" s="54"/>
+    </row>
+    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B4" s="47" t="s">
         <v>245</v>
       </c>
-      <c r="C3" s="61"/>
-      <c r="D3" s="62"/>
-      <c r="E3" s="62"/>
-      <c r="F3" s="63"/>
-    </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B4" s="54" t="s">
+      <c r="C4" s="52"/>
+      <c r="D4" s="53"/>
+      <c r="E4" s="53"/>
+      <c r="F4" s="54"/>
+    </row>
+    <row r="5" spans="2:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="B5" s="47" t="s">
         <v>246</v>
       </c>
-      <c r="C4" s="61"/>
-      <c r="D4" s="62"/>
-      <c r="E4" s="62"/>
-      <c r="F4" s="63"/>
-    </row>
-    <row r="5" spans="2:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="B5" s="54" t="s">
+      <c r="C5" s="52"/>
+      <c r="D5" s="53"/>
+      <c r="E5" s="53"/>
+      <c r="F5" s="54"/>
+    </row>
+    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B8" s="48" t="s">
         <v>247</v>
       </c>
-      <c r="C5" s="61"/>
-      <c r="D5" s="62"/>
-      <c r="E5" s="62"/>
-      <c r="F5" s="63"/>
-    </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B8" s="55" t="s">
+      <c r="C8" s="48" t="s">
         <v>248</v>
       </c>
-      <c r="C8" s="55" t="s">
+      <c r="D8" s="48" t="s">
         <v>249</v>
       </c>
-      <c r="D8" s="55" t="s">
+      <c r="E8" s="48" t="s">
         <v>250</v>
       </c>
-      <c r="E8" s="55" t="s">
+      <c r="F8" s="48" t="s">
         <v>251</v>
       </c>
-      <c r="F8" s="55" t="s">
-        <v>252</v>
-      </c>
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B9" s="53">
+      <c r="B9" s="46">
         <v>1</v>
       </c>
-      <c r="C9" s="53" t="s">
-        <v>253</v>
-      </c>
-      <c r="D9" s="56" t="s">
-        <v>253</v>
-      </c>
-      <c r="E9" s="53"/>
-      <c r="F9" s="53"/>
+      <c r="C9" s="46" t="s">
+        <v>261</v>
+      </c>
+      <c r="D9" s="80" t="s">
+        <v>261</v>
+      </c>
+      <c r="E9" s="46"/>
+      <c r="F9" s="46"/>
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B10" s="53">
+      <c r="B10" s="46">
         <v>2</v>
       </c>
-      <c r="C10" s="53" t="s">
-        <v>254</v>
-      </c>
-      <c r="D10" s="56" t="s">
-        <v>254</v>
-      </c>
-      <c r="E10" s="53"/>
-      <c r="F10" s="53"/>
+      <c r="C10" s="46" t="s">
+        <v>262</v>
+      </c>
+      <c r="D10" s="80" t="s">
+        <v>262</v>
+      </c>
+      <c r="E10" s="46"/>
+      <c r="F10" s="46"/>
     </row>
     <row r="11" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B11" s="53">
+      <c r="B11" s="46">
         <v>3</v>
       </c>
-      <c r="C11" s="53"/>
-      <c r="D11" s="53" t="s">
-        <v>264</v>
-      </c>
-      <c r="E11" s="53"/>
-      <c r="F11" s="53"/>
+      <c r="C11" s="46"/>
+      <c r="D11" s="46"/>
+      <c r="E11" s="46"/>
+      <c r="F11" s="46"/>
     </row>
     <row r="12" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B12" s="53">
+      <c r="B12" s="46">
         <v>4</v>
       </c>
-      <c r="C12" s="53"/>
-      <c r="D12" s="53"/>
-      <c r="E12" s="53"/>
-      <c r="F12" s="53"/>
+      <c r="C12" s="46"/>
+      <c r="D12" s="46"/>
+      <c r="E12" s="46"/>
+      <c r="F12" s="46"/>
     </row>
     <row r="13" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B13" s="53">
+      <c r="B13" s="46">
         <v>5</v>
       </c>
-      <c r="C13" s="53"/>
-      <c r="D13" s="53"/>
-      <c r="E13" s="53"/>
-      <c r="F13" s="53"/>
+      <c r="C13" s="46"/>
+      <c r="D13" s="46"/>
+      <c r="E13" s="46"/>
+      <c r="F13" s="46"/>
     </row>
     <row r="14" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B14" s="53">
+      <c r="B14" s="46">
         <v>6</v>
       </c>
-      <c r="C14" s="53"/>
-      <c r="D14" s="53"/>
-      <c r="E14" s="53"/>
-      <c r="F14" s="53"/>
+      <c r="C14" s="46"/>
+      <c r="D14" s="46"/>
+      <c r="E14" s="46"/>
+      <c r="F14" s="46"/>
     </row>
     <row r="15" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B15" s="53">
+      <c r="B15" s="46">
         <v>7</v>
       </c>
-      <c r="C15" s="53"/>
-      <c r="D15" s="53"/>
-      <c r="E15" s="53"/>
-      <c r="F15" s="53"/>
+      <c r="C15" s="46"/>
+      <c r="D15" s="46"/>
+      <c r="E15" s="46"/>
+      <c r="F15" s="46"/>
     </row>
     <row r="16" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B16" s="53">
+      <c r="B16" s="46">
         <v>8</v>
       </c>
-      <c r="C16" s="53"/>
-      <c r="D16" s="53"/>
-      <c r="E16" s="53"/>
-      <c r="F16" s="53"/>
+      <c r="C16" s="46"/>
+      <c r="D16" s="46"/>
+      <c r="E16" s="46"/>
+      <c r="F16" s="46"/>
     </row>
     <row r="17" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B17" s="53">
+      <c r="B17" s="46">
         <v>9</v>
       </c>
-      <c r="C17" s="53"/>
-      <c r="D17" s="53"/>
-      <c r="E17" s="53"/>
-      <c r="F17" s="53"/>
+      <c r="C17" s="46"/>
+      <c r="D17" s="46"/>
+      <c r="E17" s="46"/>
+      <c r="F17" s="46"/>
     </row>
     <row r="18" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B18" s="53">
+      <c r="B18" s="46">
         <v>10</v>
       </c>
-      <c r="C18" s="53"/>
-      <c r="D18" s="53"/>
-      <c r="E18" s="53"/>
-      <c r="F18" s="53"/>
+      <c r="C18" s="46"/>
+      <c r="D18" s="46"/>
+      <c r="E18" s="46"/>
+      <c r="F18" s="46"/>
     </row>
     <row r="19" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B19" s="53">
+      <c r="B19" s="46">
         <v>11</v>
       </c>
-      <c r="C19" s="53"/>
-      <c r="D19" s="53"/>
-      <c r="E19" s="53"/>
-      <c r="F19" s="53"/>
+      <c r="C19" s="46"/>
+      <c r="D19" s="46"/>
+      <c r="E19" s="46"/>
+      <c r="F19" s="46"/>
     </row>
     <row r="20" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B20" s="53">
+      <c r="B20" s="46">
         <v>12</v>
       </c>
-      <c r="C20" s="53"/>
-      <c r="D20" s="53"/>
-      <c r="E20" s="53"/>
-      <c r="F20" s="53"/>
+      <c r="C20" s="46"/>
+      <c r="D20" s="46"/>
+      <c r="E20" s="46"/>
+      <c r="F20" s="46"/>
     </row>
     <row r="21" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B21" s="53">
+      <c r="B21" s="46">
         <v>13</v>
       </c>
-      <c r="C21" s="53"/>
-      <c r="D21" s="53"/>
-      <c r="E21" s="53"/>
-      <c r="F21" s="53"/>
+      <c r="C21" s="46"/>
+      <c r="D21" s="46"/>
+      <c r="E21" s="46"/>
+      <c r="F21" s="46"/>
     </row>
     <row r="22" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B22" s="53">
+      <c r="B22" s="46">
         <v>14</v>
       </c>
-      <c r="C22" s="53"/>
-      <c r="D22" s="53"/>
-      <c r="E22" s="53"/>
-      <c r="F22" s="53"/>
+      <c r="C22" s="46"/>
+      <c r="D22" s="46"/>
+      <c r="E22" s="46"/>
+      <c r="F22" s="46"/>
     </row>
     <row r="23" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B23" s="53">
+      <c r="B23" s="46">
         <v>15</v>
       </c>
-      <c r="C23" s="53"/>
-      <c r="D23" s="53"/>
-      <c r="E23" s="53"/>
-      <c r="F23" s="53"/>
+      <c r="C23" s="46"/>
+      <c r="D23" s="46"/>
+      <c r="E23" s="46"/>
+      <c r="F23" s="46"/>
     </row>
     <row r="24" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B24" s="53">
+      <c r="B24" s="46">
         <v>16</v>
       </c>
-      <c r="C24" s="53"/>
-      <c r="D24" s="53"/>
-      <c r="E24" s="53"/>
-      <c r="F24" s="53"/>
+      <c r="C24" s="46"/>
+      <c r="D24" s="46"/>
+      <c r="E24" s="46"/>
+      <c r="F24" s="46"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -2037,8 +2112,8 @@
     <mergeCell ref="C3:F3"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="D9" location="Login!A1" display="Register" xr:uid="{EB027597-9839-4D29-AC7A-847681C5F9DA}"/>
-    <hyperlink ref="D10" location="Register!A1" display="Login" xr:uid="{7207D06D-AC60-46CB-987C-ABDF9D17AAFC}"/>
+    <hyperlink ref="D9" location="'Đăng ký'!A1" display="Đăng ký " xr:uid="{2F420103-D609-4867-BBE0-C84CEA6F50D4}"/>
+    <hyperlink ref="D10" location="'Đăng nhập'!A1" display="Đăng nhập" xr:uid="{B2CB2630-AD9E-450C-9EE7-09D0E3849BB2}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2049,10 +2124,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K39"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="7" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="7" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="C1" sqref="C1"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2073,53 +2148,53 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="32" t="s">
-        <v>123</v>
-      </c>
-      <c r="B1" s="73" t="s">
-        <v>129</v>
-      </c>
-      <c r="C1" s="74"/>
-      <c r="D1" s="74"/>
-      <c r="E1" s="75"/>
+        <v>122</v>
+      </c>
+      <c r="B1" s="61" t="s">
+        <v>128</v>
+      </c>
+      <c r="C1" s="62"/>
+      <c r="D1" s="62"/>
+      <c r="E1" s="63"/>
       <c r="F1" s="12"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="32" t="s">
-        <v>124</v>
-      </c>
-      <c r="B2" s="70"/>
-      <c r="C2" s="71"/>
-      <c r="D2" s="71"/>
-      <c r="E2" s="72"/>
+        <v>123</v>
+      </c>
+      <c r="B2" s="58"/>
+      <c r="C2" s="59"/>
+      <c r="D2" s="59"/>
+      <c r="E2" s="60"/>
       <c r="F2" s="12"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="32" t="s">
-        <v>125</v>
-      </c>
-      <c r="B3" s="67" t="s">
-        <v>130</v>
-      </c>
-      <c r="C3" s="68"/>
-      <c r="D3" s="68"/>
-      <c r="E3" s="69"/>
+        <v>124</v>
+      </c>
+      <c r="B3" s="55" t="s">
+        <v>129</v>
+      </c>
+      <c r="C3" s="56"/>
+      <c r="D3" s="56"/>
+      <c r="E3" s="57"/>
       <c r="F3" s="27"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="32" t="s">
+        <v>125</v>
+      </c>
+      <c r="B4" s="29" t="s">
         <v>126</v>
       </c>
-      <c r="B4" s="29" t="s">
+      <c r="C4" s="29" t="s">
+        <v>97</v>
+      </c>
+      <c r="D4" s="30" t="s">
         <v>127</v>
       </c>
-      <c r="C4" s="29" t="s">
-        <v>98</v>
-      </c>
-      <c r="D4" s="30" t="s">
-        <v>128</v>
-      </c>
       <c r="E4" s="30" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="F4" s="31"/>
     </row>
@@ -2185,23 +2260,23 @@
       <c r="A8" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="65" t="s">
+      <c r="B8" s="64" t="s">
         <v>29</v>
       </c>
       <c r="C8" s="19" t="s">
         <v>30</v>
       </c>
       <c r="D8" s="20" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E8" s="20"/>
       <c r="F8" s="21" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G8" s="20"/>
       <c r="H8" s="20"/>
       <c r="I8" s="22" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J8" s="20"/>
       <c r="K8" s="20"/>
@@ -2210,21 +2285,21 @@
       <c r="A9" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="65"/>
+      <c r="B9" s="64"/>
       <c r="C9" s="19" t="s">
-        <v>31</v>
+        <v>299</v>
       </c>
       <c r="D9" s="20" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E9" s="20"/>
       <c r="F9" s="21" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G9" s="20"/>
       <c r="H9" s="20"/>
       <c r="I9" s="22" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J9" s="20"/>
       <c r="K9" s="20"/>
@@ -2233,25 +2308,25 @@
       <c r="A10" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="B10" s="65" t="s">
-        <v>37</v>
+      <c r="B10" s="64" t="s">
+        <v>36</v>
       </c>
       <c r="C10" s="19"/>
       <c r="D10" s="20" t="s">
-        <v>38</v>
-      </c>
-      <c r="E10" s="65" t="s">
-        <v>46</v>
+        <v>37</v>
+      </c>
+      <c r="E10" s="64" t="s">
+        <v>45</v>
       </c>
       <c r="F10" s="21" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G10" s="20"/>
       <c r="H10" s="20" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="I10" s="22" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J10" s="20"/>
       <c r="K10" s="20"/>
@@ -2260,21 +2335,21 @@
       <c r="A11" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="B11" s="65"/>
+      <c r="B11" s="64"/>
       <c r="C11" s="19"/>
       <c r="D11" s="20" t="s">
-        <v>39</v>
-      </c>
-      <c r="E11" s="65"/>
+        <v>38</v>
+      </c>
+      <c r="E11" s="64"/>
       <c r="F11" s="21" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G11" s="20"/>
       <c r="H11" s="20" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="I11" s="22" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J11" s="20"/>
       <c r="K11" s="20"/>
@@ -2283,21 +2358,21 @@
       <c r="A12" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="B12" s="65"/>
+      <c r="B12" s="64"/>
       <c r="C12" s="19"/>
       <c r="D12" s="20" t="s">
-        <v>40</v>
-      </c>
-      <c r="E12" s="65"/>
+        <v>39</v>
+      </c>
+      <c r="E12" s="64"/>
       <c r="F12" s="21" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G12" s="20"/>
       <c r="H12" s="20" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="I12" s="22" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J12" s="20"/>
       <c r="K12" s="20"/>
@@ -2306,21 +2381,21 @@
       <c r="A13" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="B13" s="65"/>
+      <c r="B13" s="64"/>
       <c r="C13" s="19"/>
       <c r="D13" s="20" t="s">
-        <v>41</v>
-      </c>
-      <c r="E13" s="65"/>
+        <v>40</v>
+      </c>
+      <c r="E13" s="64"/>
       <c r="F13" s="21" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G13" s="20"/>
       <c r="H13" s="20" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="I13" s="22" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J13" s="20"/>
       <c r="K13" s="20"/>
@@ -2329,21 +2404,21 @@
       <c r="A14" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="B14" s="65"/>
+      <c r="B14" s="64"/>
       <c r="C14" s="19"/>
       <c r="D14" s="20" t="s">
-        <v>47</v>
-      </c>
-      <c r="E14" s="65"/>
+        <v>46</v>
+      </c>
+      <c r="E14" s="64"/>
       <c r="F14" s="21" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G14" s="20"/>
       <c r="H14" s="20" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="I14" s="22" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J14" s="20"/>
       <c r="K14" s="20"/>
@@ -2352,29 +2427,29 @@
       <c r="A15" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="B15" s="65" t="s">
+      <c r="B15" s="64" t="s">
+        <v>53</v>
+      </c>
+      <c r="C15" s="64" t="s">
         <v>54</v>
       </c>
-      <c r="C15" s="65" t="s">
+      <c r="D15" s="20" t="s">
+        <v>63</v>
+      </c>
+      <c r="E15" s="64" t="s">
+        <v>45</v>
+      </c>
+      <c r="F15" s="65" t="s">
+        <v>72</v>
+      </c>
+      <c r="G15" s="20" t="s">
         <v>55</v>
       </c>
-      <c r="D15" s="20" t="s">
-        <v>64</v>
-      </c>
-      <c r="E15" s="65" t="s">
-        <v>46</v>
-      </c>
-      <c r="F15" s="64" t="s">
-        <v>73</v>
-      </c>
-      <c r="G15" s="20" t="s">
+      <c r="H15" s="65" t="s">
         <v>56</v>
       </c>
-      <c r="H15" s="64" t="s">
-        <v>57</v>
-      </c>
       <c r="I15" s="22" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J15" s="20"/>
       <c r="K15" s="20"/>
@@ -2383,19 +2458,19 @@
       <c r="A16" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="B16" s="65"/>
-      <c r="C16" s="65"/>
+      <c r="B16" s="64"/>
+      <c r="C16" s="64"/>
       <c r="D16" s="20" t="s">
+        <v>64</v>
+      </c>
+      <c r="E16" s="64"/>
+      <c r="F16" s="65"/>
+      <c r="G16" s="20" t="s">
         <v>65</v>
       </c>
-      <c r="E16" s="65"/>
-      <c r="F16" s="64"/>
-      <c r="G16" s="20" t="s">
-        <v>66</v>
-      </c>
-      <c r="H16" s="64"/>
+      <c r="H16" s="65"/>
       <c r="I16" s="22" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J16" s="20"/>
       <c r="K16" s="20"/>
@@ -2404,23 +2479,23 @@
       <c r="A17" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="B17" s="65"/>
-      <c r="C17" s="65"/>
+      <c r="B17" s="64"/>
+      <c r="C17" s="64"/>
       <c r="D17" s="20" t="s">
+        <v>57</v>
+      </c>
+      <c r="E17" s="64"/>
+      <c r="F17" s="65" t="s">
         <v>58</v>
       </c>
-      <c r="E17" s="65"/>
-      <c r="F17" s="64" t="s">
+      <c r="G17" s="20" t="s">
         <v>59</v>
       </c>
-      <c r="G17" s="20" t="s">
+      <c r="H17" s="65" t="s">
         <v>60</v>
       </c>
-      <c r="H17" s="64" t="s">
-        <v>61</v>
-      </c>
       <c r="I17" s="22" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J17" s="20"/>
       <c r="K17" s="20"/>
@@ -2429,19 +2504,19 @@
       <c r="A18" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="B18" s="65"/>
-      <c r="C18" s="65"/>
+      <c r="B18" s="64"/>
+      <c r="C18" s="64"/>
       <c r="D18" s="20" t="s">
-        <v>63</v>
-      </c>
-      <c r="E18" s="65"/>
-      <c r="F18" s="64"/>
+        <v>62</v>
+      </c>
+      <c r="E18" s="64"/>
+      <c r="F18" s="65"/>
       <c r="G18" s="20" t="s">
-        <v>62</v>
-      </c>
-      <c r="H18" s="64"/>
+        <v>61</v>
+      </c>
+      <c r="H18" s="65"/>
       <c r="I18" s="22" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J18" s="20"/>
       <c r="K18" s="20"/>
@@ -2450,21 +2525,21 @@
       <c r="A19" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="B19" s="65"/>
-      <c r="C19" s="65"/>
+      <c r="B19" s="64"/>
+      <c r="C19" s="64"/>
       <c r="D19" s="20" t="s">
+        <v>66</v>
+      </c>
+      <c r="E19" s="64"/>
+      <c r="F19" s="65"/>
+      <c r="G19" s="20" t="s">
         <v>67</v>
       </c>
-      <c r="E19" s="65"/>
-      <c r="F19" s="64"/>
-      <c r="G19" s="20" t="s">
+      <c r="H19" s="20" t="s">
         <v>68</v>
       </c>
-      <c r="H19" s="20" t="s">
-        <v>69</v>
-      </c>
       <c r="I19" s="22" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J19" s="20"/>
       <c r="K19" s="20"/>
@@ -2473,23 +2548,23 @@
       <c r="A20" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="B20" s="65"/>
-      <c r="C20" s="65"/>
+      <c r="B20" s="64"/>
+      <c r="C20" s="64"/>
       <c r="D20" s="20" t="s">
+        <v>69</v>
+      </c>
+      <c r="E20" s="64"/>
+      <c r="F20" s="21" t="s">
+        <v>72</v>
+      </c>
+      <c r="G20" s="20" t="s">
         <v>70</v>
       </c>
-      <c r="E20" s="65"/>
-      <c r="F20" s="21" t="s">
-        <v>73</v>
-      </c>
-      <c r="G20" s="20" t="s">
+      <c r="H20" s="20" t="s">
         <v>71</v>
       </c>
-      <c r="H20" s="20" t="s">
-        <v>72</v>
-      </c>
       <c r="I20" s="22" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J20" s="20"/>
       <c r="K20" s="20"/>
@@ -2498,27 +2573,27 @@
       <c r="A21" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="B21" s="65"/>
-      <c r="C21" s="65" t="s">
-        <v>74</v>
+      <c r="B21" s="64"/>
+      <c r="C21" s="64" t="s">
+        <v>73</v>
       </c>
       <c r="D21" s="20" t="s">
-        <v>85</v>
-      </c>
-      <c r="E21" s="65" t="s">
-        <v>46</v>
+        <v>84</v>
+      </c>
+      <c r="E21" s="64" t="s">
+        <v>45</v>
       </c>
       <c r="F21" s="21" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G21" s="20" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="H21" s="20" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="I21" s="22" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J21" s="20"/>
       <c r="K21" s="20"/>
@@ -2527,23 +2602,23 @@
       <c r="A22" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="B22" s="65"/>
-      <c r="C22" s="65"/>
+      <c r="B22" s="64"/>
+      <c r="C22" s="64"/>
       <c r="D22" s="20" t="s">
+        <v>74</v>
+      </c>
+      <c r="E22" s="64"/>
+      <c r="F22" s="21" t="s">
         <v>75</v>
       </c>
-      <c r="E22" s="65"/>
-      <c r="F22" s="21" t="s">
+      <c r="G22" s="20" t="s">
         <v>76</v>
       </c>
-      <c r="G22" s="20" t="s">
-        <v>77</v>
-      </c>
       <c r="H22" s="20" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="I22" s="22" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J22" s="20"/>
       <c r="K22" s="20"/>
@@ -2552,23 +2627,23 @@
       <c r="A23" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="B23" s="65"/>
-      <c r="C23" s="65"/>
+      <c r="B23" s="64"/>
+      <c r="C23" s="64"/>
       <c r="D23" s="20" t="s">
+        <v>77</v>
+      </c>
+      <c r="E23" s="64"/>
+      <c r="F23" s="65" t="s">
         <v>78</v>
       </c>
-      <c r="E23" s="65"/>
-      <c r="F23" s="64" t="s">
+      <c r="G23" s="20" t="s">
+        <v>80</v>
+      </c>
+      <c r="H23" s="23" t="s">
         <v>79</v>
       </c>
-      <c r="G23" s="20" t="s">
-        <v>81</v>
-      </c>
-      <c r="H23" s="23" t="s">
-        <v>80</v>
-      </c>
       <c r="I23" s="22" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J23" s="20"/>
       <c r="K23" s="20"/>
@@ -2577,21 +2652,21 @@
       <c r="A24" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="B24" s="65"/>
-      <c r="C24" s="65"/>
+      <c r="B24" s="64"/>
+      <c r="C24" s="64"/>
       <c r="D24" s="20" t="s">
+        <v>81</v>
+      </c>
+      <c r="E24" s="64"/>
+      <c r="F24" s="65"/>
+      <c r="G24" s="20" t="s">
         <v>82</v>
       </c>
-      <c r="E24" s="65"/>
-      <c r="F24" s="64"/>
-      <c r="G24" s="20" t="s">
-        <v>83</v>
-      </c>
       <c r="H24" s="20" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="I24" s="22" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J24" s="20"/>
       <c r="K24" s="20"/>
@@ -2600,29 +2675,29 @@
       <c r="A25" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="B25" s="65" t="s">
+      <c r="B25" s="64" t="s">
+        <v>85</v>
+      </c>
+      <c r="C25" s="64" t="s">
+        <v>90</v>
+      </c>
+      <c r="D25" s="20" t="s">
         <v>86</v>
       </c>
-      <c r="C25" s="65" t="s">
-        <v>91</v>
-      </c>
-      <c r="D25" s="20" t="s">
+      <c r="E25" s="65" t="s">
+        <v>45</v>
+      </c>
+      <c r="F25" s="66" t="s">
+        <v>75</v>
+      </c>
+      <c r="G25" s="20" t="s">
         <v>87</v>
       </c>
-      <c r="E25" s="64" t="s">
-        <v>46</v>
-      </c>
-      <c r="F25" s="66" t="s">
-        <v>76</v>
-      </c>
-      <c r="G25" s="20" t="s">
-        <v>88</v>
-      </c>
       <c r="H25" s="20" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="I25" s="22" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J25" s="20"/>
       <c r="K25" s="20"/>
@@ -2631,192 +2706,192 @@
       <c r="A26" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="B26" s="65"/>
-      <c r="C26" s="65"/>
+      <c r="B26" s="64"/>
+      <c r="C26" s="64"/>
       <c r="D26" s="20" t="s">
-        <v>89</v>
-      </c>
-      <c r="E26" s="64"/>
+        <v>88</v>
+      </c>
+      <c r="E26" s="65"/>
       <c r="F26" s="66"/>
       <c r="G26" s="20" t="s">
-        <v>90</v>
-      </c>
-      <c r="H26" s="64" t="s">
-        <v>72</v>
+        <v>89</v>
+      </c>
+      <c r="H26" s="65" t="s">
+        <v>71</v>
       </c>
       <c r="I26" s="22" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J26" s="20"/>
       <c r="K26" s="20"/>
     </row>
     <row r="27" spans="1:11" ht="56.25" x14ac:dyDescent="0.25">
       <c r="A27" s="18" t="s">
-        <v>116</v>
-      </c>
-      <c r="B27" s="65"/>
-      <c r="C27" s="65"/>
+        <v>115</v>
+      </c>
+      <c r="B27" s="64"/>
+      <c r="C27" s="64"/>
       <c r="D27" s="20" t="s">
-        <v>92</v>
-      </c>
-      <c r="E27" s="64"/>
+        <v>91</v>
+      </c>
+      <c r="E27" s="65"/>
       <c r="F27" s="66"/>
       <c r="G27" s="20" t="s">
-        <v>93</v>
-      </c>
-      <c r="H27" s="64"/>
+        <v>92</v>
+      </c>
+      <c r="H27" s="65"/>
       <c r="I27" s="22" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J27" s="20"/>
       <c r="K27" s="20"/>
     </row>
     <row r="28" spans="1:11" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A28" s="18" t="s">
-        <v>117</v>
-      </c>
-      <c r="B28" s="65"/>
+        <v>116</v>
+      </c>
+      <c r="B28" s="64"/>
       <c r="C28" s="22" t="s">
+        <v>105</v>
+      </c>
+      <c r="D28" s="20" t="s">
         <v>106</v>
       </c>
-      <c r="D28" s="20" t="s">
+      <c r="E28" s="64" t="s">
+        <v>45</v>
+      </c>
+      <c r="F28" s="19" t="s">
         <v>107</v>
-      </c>
-      <c r="E28" s="65" t="s">
-        <v>46</v>
-      </c>
-      <c r="F28" s="19" t="s">
-        <v>108</v>
       </c>
       <c r="G28" s="20"/>
       <c r="H28" s="24" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="I28" s="22" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J28" s="20"/>
       <c r="K28" s="20"/>
     </row>
     <row r="29" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A29" s="18" t="s">
-        <v>118</v>
-      </c>
-      <c r="B29" s="65"/>
-      <c r="C29" s="65" t="s">
-        <v>94</v>
+        <v>117</v>
+      </c>
+      <c r="B29" s="64"/>
+      <c r="C29" s="64" t="s">
+        <v>93</v>
       </c>
       <c r="D29" s="20" t="s">
-        <v>96</v>
-      </c>
-      <c r="E29" s="65"/>
+        <v>95</v>
+      </c>
+      <c r="E29" s="64"/>
       <c r="F29" s="21" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="G29" s="20"/>
       <c r="H29" s="19" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="I29" s="22" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J29" s="20"/>
       <c r="K29" s="20"/>
     </row>
     <row r="30" spans="1:11" ht="37.5" x14ac:dyDescent="0.3">
       <c r="A30" s="18" t="s">
-        <v>119</v>
-      </c>
-      <c r="B30" s="65"/>
-      <c r="C30" s="65"/>
+        <v>118</v>
+      </c>
+      <c r="B30" s="64"/>
+      <c r="C30" s="64"/>
       <c r="D30" s="21" t="s">
-        <v>97</v>
-      </c>
-      <c r="E30" s="65"/>
+        <v>96</v>
+      </c>
+      <c r="E30" s="64"/>
       <c r="F30" s="23" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="G30" s="25"/>
       <c r="H30" s="19" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="I30" s="22" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J30" s="25"/>
       <c r="K30" s="25"/>
     </row>
     <row r="31" spans="1:11" ht="56.25" x14ac:dyDescent="0.3">
       <c r="A31" s="18" t="s">
-        <v>120</v>
-      </c>
-      <c r="B31" s="65"/>
-      <c r="C31" s="65" t="s">
+        <v>119</v>
+      </c>
+      <c r="B31" s="64"/>
+      <c r="C31" s="64" t="s">
+        <v>98</v>
+      </c>
+      <c r="D31" s="26" t="s">
         <v>99</v>
-      </c>
-      <c r="D31" s="26" t="s">
-        <v>100</v>
       </c>
       <c r="E31" s="25"/>
       <c r="F31" s="21" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G31" s="25"/>
       <c r="H31" s="25" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="I31" s="22" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J31" s="25"/>
       <c r="K31" s="25"/>
     </row>
     <row r="32" spans="1:11" ht="112.5" x14ac:dyDescent="0.3">
       <c r="A32" s="18" t="s">
-        <v>121</v>
-      </c>
-      <c r="B32" s="65"/>
-      <c r="C32" s="65"/>
+        <v>120</v>
+      </c>
+      <c r="B32" s="64"/>
+      <c r="C32" s="64"/>
       <c r="D32" s="19" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E32" s="25"/>
       <c r="F32" s="21" t="s">
+        <v>103</v>
+      </c>
+      <c r="G32" s="20" t="s">
+        <v>102</v>
+      </c>
+      <c r="H32" s="19" t="s">
         <v>104</v>
       </c>
-      <c r="G32" s="20" t="s">
-        <v>103</v>
-      </c>
-      <c r="H32" s="19" t="s">
-        <v>105</v>
-      </c>
       <c r="I32" s="22" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="J32" s="25"/>
       <c r="K32" s="25"/>
     </row>
     <row r="33" spans="1:11" ht="93.75" x14ac:dyDescent="0.3">
       <c r="A33" s="18" t="s">
-        <v>122</v>
-      </c>
-      <c r="B33" s="65"/>
-      <c r="C33" s="65"/>
+        <v>121</v>
+      </c>
+      <c r="B33" s="64"/>
+      <c r="C33" s="64"/>
       <c r="D33" s="19" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E33" s="25"/>
       <c r="F33" s="21" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="G33" s="20" t="s">
+        <v>113</v>
+      </c>
+      <c r="H33" s="20" t="s">
         <v>114</v>
       </c>
-      <c r="H33" s="20" t="s">
-        <v>115</v>
-      </c>
       <c r="I33" s="22" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J33" s="25"/>
       <c r="K33" s="25"/>
@@ -2901,6 +2976,19 @@
     </row>
   </sheetData>
   <mergeCells count="24">
+    <mergeCell ref="H15:H16"/>
+    <mergeCell ref="E15:E20"/>
+    <mergeCell ref="C15:C20"/>
+    <mergeCell ref="F15:F16"/>
+    <mergeCell ref="F17:F19"/>
+    <mergeCell ref="F25:F27"/>
+    <mergeCell ref="H26:H27"/>
+    <mergeCell ref="C29:C30"/>
+    <mergeCell ref="E28:E30"/>
+    <mergeCell ref="H17:H18"/>
+    <mergeCell ref="F23:F24"/>
+    <mergeCell ref="C21:C24"/>
+    <mergeCell ref="E21:E24"/>
     <mergeCell ref="B3:E3"/>
     <mergeCell ref="B2:E2"/>
     <mergeCell ref="B1:E1"/>
@@ -2912,29 +3000,16 @@
     <mergeCell ref="E10:E14"/>
     <mergeCell ref="B10:B14"/>
     <mergeCell ref="B15:B24"/>
-    <mergeCell ref="F25:F27"/>
-    <mergeCell ref="H26:H27"/>
-    <mergeCell ref="C29:C30"/>
-    <mergeCell ref="E28:E30"/>
-    <mergeCell ref="H17:H18"/>
-    <mergeCell ref="F23:F24"/>
-    <mergeCell ref="C21:C24"/>
-    <mergeCell ref="E21:E24"/>
-    <mergeCell ref="H15:H16"/>
-    <mergeCell ref="E15:E20"/>
-    <mergeCell ref="C15:C20"/>
-    <mergeCell ref="F15:F16"/>
-    <mergeCell ref="F17:F19"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="I8:I38">
-    <cfRule type="containsText" dxfId="8" priority="1" operator="containsText" text="Untested">
+    <cfRule type="containsText" dxfId="11" priority="1" operator="containsText" text="Untested">
       <formula>NOT(ISERROR(SEARCH("Untested",I8)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="7" priority="2" operator="containsText" text="Passed">
+    <cfRule type="containsText" dxfId="10" priority="2" operator="containsText" text="Passed">
       <formula>NOT(ISERROR(SEARCH("Passed",I8)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="6" priority="3" operator="containsText" text="Failed">
+    <cfRule type="containsText" dxfId="9" priority="3" operator="containsText" text="Failed">
       <formula>NOT(ISERROR(SEARCH("Failed",I8)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2952,9 +3027,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D522390-3A2F-4FA6-BCAD-19EE22305088}">
   <dimension ref="A1:K42"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="7" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D9" sqref="D9"/>
+      <selection pane="bottomLeft" activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2974,77 +3049,77 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="57" t="s">
+      <c r="A1" s="83" t="s">
+        <v>122</v>
+      </c>
+      <c r="B1" s="81" t="s">
+        <v>242</v>
+      </c>
+      <c r="C1" s="81"/>
+      <c r="D1" s="81"/>
+      <c r="E1" s="81"/>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="83" t="s">
         <v>123</v>
       </c>
-      <c r="B1" s="84" t="s">
-        <v>243</v>
-      </c>
-      <c r="C1" s="84"/>
-      <c r="D1" s="84"/>
-      <c r="E1" s="84"/>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="57" t="s">
+      <c r="B2" s="77"/>
+      <c r="C2" s="77"/>
+      <c r="D2" s="77"/>
+      <c r="E2" s="77"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" s="83" t="s">
         <v>124</v>
       </c>
-      <c r="B2" s="85"/>
-      <c r="C2" s="85"/>
-      <c r="D2" s="85"/>
-      <c r="E2" s="85"/>
-    </row>
-    <row r="3" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="57" t="s">
+      <c r="B3" s="82" t="s">
+        <v>129</v>
+      </c>
+      <c r="C3" s="82"/>
+      <c r="D3" s="82"/>
+      <c r="E3" s="82"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" s="83" t="s">
         <v>125</v>
       </c>
-      <c r="B3" s="86" t="s">
-        <v>130</v>
-      </c>
-      <c r="C3" s="86"/>
-      <c r="D3" s="86"/>
-      <c r="E3" s="86"/>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="58" t="s">
+      <c r="B4" s="50" t="s">
         <v>126</v>
       </c>
-      <c r="B4" s="48" t="s">
+      <c r="C4" s="50" t="s">
+        <v>97</v>
+      </c>
+      <c r="D4" s="30" t="s">
         <v>127</v>
       </c>
-      <c r="C4" s="48" t="s">
-        <v>98</v>
-      </c>
-      <c r="D4" s="49" t="s">
-        <v>128</v>
-      </c>
-      <c r="E4" s="50" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="59">
+      <c r="E4" s="30" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" s="50">
         <f>COUNTA(I8:I42)</f>
         <v>35</v>
       </c>
-      <c r="B5" s="45">
+      <c r="B5" s="50">
         <f>COUNTIF(I8:I42,I8)</f>
         <v>33</v>
       </c>
-      <c r="C5" s="45">
+      <c r="C5" s="50">
         <f>COUNTIF(I8:I42,"Failed")</f>
         <v>2</v>
       </c>
-      <c r="D5" s="46">
+      <c r="D5" s="30">
         <f>COUNTIF(I8:I42,"Untested")</f>
         <v>0</v>
       </c>
-      <c r="E5" s="47">
+      <c r="E5" s="30">
         <f>COUNTIF(I8:I42,"N/A")</f>
         <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:11" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A6" s="60"/>
+      <c r="A6" s="49"/>
       <c r="C6" s="42"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
@@ -3084,7 +3159,7 @@
     </row>
     <row r="8" spans="1:11" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A8" s="41" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B8" s="35" t="s">
         <v>29</v>
@@ -3093,864 +3168,877 @@
         <v>30</v>
       </c>
       <c r="D8" s="36" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E8" s="36" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F8" s="37" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="G8" s="36"/>
       <c r="H8" s="36" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="I8" s="41" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J8" s="36"/>
       <c r="K8" s="36"/>
     </row>
     <row r="9" spans="1:11" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A9" s="41" t="s">
-        <v>263</v>
-      </c>
-      <c r="B9" s="81" t="s">
-        <v>37</v>
+        <v>260</v>
+      </c>
+      <c r="B9" s="76" t="s">
+        <v>36</v>
       </c>
       <c r="C9" s="41"/>
       <c r="D9" s="36" t="s">
-        <v>38</v>
-      </c>
-      <c r="E9" s="82" t="s">
-        <v>167</v>
+        <v>37</v>
+      </c>
+      <c r="E9" s="77" t="s">
+        <v>166</v>
       </c>
       <c r="F9" s="37" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G9" s="36"/>
       <c r="H9" s="36" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="I9" s="41" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J9" s="36"/>
       <c r="K9" s="36"/>
     </row>
     <row r="10" spans="1:11" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A10" s="41" t="s">
-        <v>132</v>
-      </c>
-      <c r="B10" s="81"/>
+        <v>131</v>
+      </c>
+      <c r="B10" s="76"/>
       <c r="C10" s="41"/>
       <c r="D10" s="36" t="s">
-        <v>39</v>
-      </c>
-      <c r="E10" s="82"/>
+        <v>38</v>
+      </c>
+      <c r="E10" s="77"/>
       <c r="F10" s="37" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G10" s="36"/>
       <c r="H10" s="36" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="I10" s="41" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J10" s="36"/>
       <c r="K10" s="36"/>
     </row>
     <row r="11" spans="1:11" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A11" s="41" t="s">
-        <v>133</v>
-      </c>
-      <c r="B11" s="81"/>
+        <v>132</v>
+      </c>
+      <c r="B11" s="76"/>
       <c r="C11" s="41"/>
       <c r="D11" s="36" t="s">
-        <v>40</v>
-      </c>
-      <c r="E11" s="82"/>
+        <v>39</v>
+      </c>
+      <c r="E11" s="77"/>
       <c r="F11" s="37" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G11" s="36"/>
       <c r="H11" s="36" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="I11" s="41" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J11" s="36"/>
       <c r="K11" s="36"/>
     </row>
     <row r="12" spans="1:11" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A12" s="41" t="s">
-        <v>134</v>
-      </c>
-      <c r="B12" s="81"/>
+        <v>133</v>
+      </c>
+      <c r="B12" s="76"/>
       <c r="C12" s="41"/>
       <c r="D12" s="36" t="s">
-        <v>41</v>
-      </c>
-      <c r="E12" s="82"/>
+        <v>40</v>
+      </c>
+      <c r="E12" s="77"/>
       <c r="F12" s="37" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G12" s="36"/>
       <c r="H12" s="36" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="I12" s="41" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J12" s="36"/>
       <c r="K12" s="36"/>
     </row>
     <row r="13" spans="1:11" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A13" s="41" t="s">
-        <v>135</v>
-      </c>
-      <c r="B13" s="81"/>
+        <v>134</v>
+      </c>
+      <c r="B13" s="76"/>
       <c r="C13" s="41"/>
       <c r="D13" s="36" t="s">
-        <v>47</v>
-      </c>
-      <c r="E13" s="82"/>
+        <v>46</v>
+      </c>
+      <c r="E13" s="77"/>
       <c r="F13" s="37" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G13" s="36"/>
       <c r="H13" s="35" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="I13" s="41" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J13" s="36"/>
       <c r="K13" s="36"/>
     </row>
     <row r="14" spans="1:11" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A14" s="41" t="s">
-        <v>136</v>
-      </c>
-      <c r="B14" s="78" t="s">
+        <v>135</v>
+      </c>
+      <c r="B14" s="67" t="s">
+        <v>161</v>
+      </c>
+      <c r="C14" s="67" t="s">
         <v>162</v>
       </c>
-      <c r="C14" s="78" t="s">
+      <c r="D14" s="35" t="s">
+        <v>165</v>
+      </c>
+      <c r="E14" s="72" t="s">
+        <v>166</v>
+      </c>
+      <c r="F14" s="37" t="s">
         <v>163</v>
       </c>
-      <c r="D14" s="35" t="s">
-        <v>166</v>
-      </c>
-      <c r="E14" s="76" t="s">
-        <v>167</v>
-      </c>
-      <c r="F14" s="37" t="s">
+      <c r="G14" s="38" t="s">
+        <v>171</v>
+      </c>
+      <c r="H14" s="35" t="s">
         <v>164</v>
       </c>
-      <c r="G14" s="38" t="s">
-        <v>172</v>
-      </c>
-      <c r="H14" s="35" t="s">
-        <v>165</v>
-      </c>
       <c r="I14" s="41" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J14" s="38"/>
       <c r="K14" s="38"/>
     </row>
     <row r="15" spans="1:11" ht="110.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="41" t="s">
-        <v>137</v>
-      </c>
-      <c r="B15" s="80"/>
-      <c r="C15" s="80"/>
+        <v>136</v>
+      </c>
+      <c r="B15" s="69"/>
+      <c r="C15" s="69"/>
       <c r="D15" s="35" t="s">
+        <v>167</v>
+      </c>
+      <c r="E15" s="73"/>
+      <c r="F15" s="72" t="s">
+        <v>187</v>
+      </c>
+      <c r="G15" s="35" t="s">
+        <v>185</v>
+      </c>
+      <c r="H15" s="35" t="s">
         <v>168</v>
       </c>
-      <c r="E15" s="83"/>
-      <c r="F15" s="76" t="s">
-        <v>188</v>
-      </c>
-      <c r="G15" s="35" t="s">
-        <v>186</v>
-      </c>
-      <c r="H15" s="35" t="s">
-        <v>169</v>
-      </c>
       <c r="I15" s="41" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J15" s="38"/>
       <c r="K15" s="38"/>
     </row>
     <row r="16" spans="1:11" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A16" s="41" t="s">
-        <v>138</v>
-      </c>
-      <c r="B16" s="80"/>
-      <c r="C16" s="79"/>
+        <v>137</v>
+      </c>
+      <c r="B16" s="69"/>
+      <c r="C16" s="68"/>
       <c r="D16" s="44" t="s">
+        <v>169</v>
+      </c>
+      <c r="E16" s="74"/>
+      <c r="F16" s="74"/>
+      <c r="G16" s="35" t="s">
+        <v>186</v>
+      </c>
+      <c r="H16" s="35" t="s">
         <v>170</v>
       </c>
-      <c r="E16" s="77"/>
-      <c r="F16" s="77"/>
-      <c r="G16" s="35" t="s">
-        <v>187</v>
-      </c>
-      <c r="H16" s="35" t="s">
-        <v>171</v>
-      </c>
       <c r="I16" s="41" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J16" s="38"/>
       <c r="K16" s="38"/>
     </row>
     <row r="17" spans="1:11" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A17" s="41" t="s">
-        <v>139</v>
-      </c>
-      <c r="B17" s="80"/>
-      <c r="C17" s="78" t="s">
+        <v>138</v>
+      </c>
+      <c r="B17" s="69"/>
+      <c r="C17" s="67" t="s">
+        <v>172</v>
+      </c>
+      <c r="D17" s="35" t="s">
+        <v>165</v>
+      </c>
+      <c r="E17" s="72" t="s">
+        <v>191</v>
+      </c>
+      <c r="F17" s="37" t="s">
         <v>173</v>
       </c>
-      <c r="D17" s="35" t="s">
-        <v>166</v>
-      </c>
-      <c r="E17" s="76" t="s">
-        <v>192</v>
-      </c>
-      <c r="F17" s="37" t="s">
+      <c r="G17" s="38" t="s">
         <v>174</v>
       </c>
-      <c r="G17" s="38" t="s">
+      <c r="H17" s="35" t="s">
         <v>175</v>
       </c>
-      <c r="H17" s="35" t="s">
-        <v>176</v>
-      </c>
       <c r="I17" s="41" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J17" s="38"/>
       <c r="K17" s="38"/>
     </row>
     <row r="18" spans="1:11" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A18" s="41" t="s">
-        <v>140</v>
-      </c>
-      <c r="B18" s="80"/>
-      <c r="C18" s="79"/>
+        <v>139</v>
+      </c>
+      <c r="B18" s="69"/>
+      <c r="C18" s="68"/>
       <c r="D18" s="35" t="s">
-        <v>261</v>
-      </c>
-      <c r="E18" s="77"/>
+        <v>258</v>
+      </c>
+      <c r="E18" s="74"/>
       <c r="F18" s="37" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="G18" s="38"/>
       <c r="H18" s="35" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="I18" s="41" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J18" s="38"/>
       <c r="K18" s="38"/>
     </row>
     <row r="19" spans="1:11" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A19" s="41" t="s">
-        <v>141</v>
-      </c>
-      <c r="B19" s="80"/>
-      <c r="C19" s="78" t="s">
+        <v>140</v>
+      </c>
+      <c r="B19" s="69"/>
+      <c r="C19" s="67" t="s">
+        <v>176</v>
+      </c>
+      <c r="D19" s="35" t="s">
+        <v>165</v>
+      </c>
+      <c r="E19" s="72" t="s">
+        <v>166</v>
+      </c>
+      <c r="F19" s="35" t="s">
         <v>177</v>
       </c>
-      <c r="D19" s="35" t="s">
-        <v>166</v>
-      </c>
-      <c r="E19" s="76" t="s">
-        <v>167</v>
-      </c>
-      <c r="F19" s="35" t="s">
+      <c r="G19" s="38" t="s">
+        <v>180</v>
+      </c>
+      <c r="H19" s="35" t="s">
         <v>178</v>
       </c>
-      <c r="G19" s="38" t="s">
-        <v>181</v>
-      </c>
-      <c r="H19" s="35" t="s">
-        <v>179</v>
-      </c>
       <c r="I19" s="41" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J19" s="38"/>
       <c r="K19" s="38"/>
     </row>
     <row r="20" spans="1:11" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A20" s="41" t="s">
-        <v>142</v>
-      </c>
-      <c r="B20" s="80"/>
-      <c r="C20" s="80"/>
+        <v>141</v>
+      </c>
+      <c r="B20" s="69"/>
+      <c r="C20" s="69"/>
       <c r="D20" s="35" t="s">
-        <v>180</v>
-      </c>
-      <c r="E20" s="83"/>
-      <c r="F20" s="78" t="s">
-        <v>191</v>
+        <v>179</v>
+      </c>
+      <c r="E20" s="73"/>
+      <c r="F20" s="67" t="s">
+        <v>190</v>
       </c>
       <c r="G20" s="35" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="H20" s="35" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="I20" s="41" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J20" s="38"/>
       <c r="K20" s="38"/>
     </row>
     <row r="21" spans="1:11" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A21" s="41" t="s">
-        <v>143</v>
-      </c>
-      <c r="B21" s="80"/>
-      <c r="C21" s="79"/>
+        <v>142</v>
+      </c>
+      <c r="B21" s="69"/>
+      <c r="C21" s="68"/>
       <c r="D21" s="35" t="s">
-        <v>183</v>
-      </c>
-      <c r="E21" s="77"/>
-      <c r="F21" s="79"/>
+        <v>182</v>
+      </c>
+      <c r="E21" s="74"/>
+      <c r="F21" s="68"/>
       <c r="G21" s="35" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="H21" s="35" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="I21" s="41" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J21" s="38"/>
       <c r="K21" s="38"/>
     </row>
     <row r="22" spans="1:11" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A22" s="41" t="s">
-        <v>144</v>
-      </c>
-      <c r="B22" s="80"/>
-      <c r="C22" s="78" t="s">
+        <v>143</v>
+      </c>
+      <c r="B22" s="69"/>
+      <c r="C22" s="67" t="s">
+        <v>198</v>
+      </c>
+      <c r="D22" s="35" t="s">
+        <v>165</v>
+      </c>
+      <c r="E22" s="72" t="s">
+        <v>166</v>
+      </c>
+      <c r="F22" s="37" t="s">
         <v>199</v>
       </c>
-      <c r="D22" s="35" t="s">
-        <v>166</v>
-      </c>
-      <c r="E22" s="76" t="s">
-        <v>167</v>
-      </c>
-      <c r="F22" s="37" t="s">
-        <v>200</v>
-      </c>
       <c r="G22" s="38" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="H22" s="35" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="I22" s="41" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J22" s="38"/>
       <c r="K22" s="38"/>
     </row>
     <row r="23" spans="1:11" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A23" s="41" t="s">
-        <v>145</v>
-      </c>
-      <c r="B23" s="80"/>
-      <c r="C23" s="80"/>
+        <v>144</v>
+      </c>
+      <c r="B23" s="69"/>
+      <c r="C23" s="69"/>
       <c r="D23" s="35" t="s">
-        <v>202</v>
-      </c>
-      <c r="E23" s="83"/>
-      <c r="F23" s="76" t="s">
         <v>201</v>
       </c>
+      <c r="E23" s="73"/>
+      <c r="F23" s="72" t="s">
+        <v>200</v>
+      </c>
       <c r="G23" s="35" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="H23" s="35" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="I23" s="41" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J23" s="38"/>
       <c r="K23" s="38"/>
     </row>
     <row r="24" spans="1:11" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A24" s="41" t="s">
-        <v>146</v>
-      </c>
-      <c r="B24" s="80"/>
-      <c r="C24" s="80"/>
+        <v>145</v>
+      </c>
+      <c r="B24" s="69"/>
+      <c r="C24" s="69"/>
       <c r="D24" s="20" t="s">
-        <v>230</v>
-      </c>
-      <c r="E24" s="83"/>
-      <c r="F24" s="83"/>
+        <v>229</v>
+      </c>
+      <c r="E24" s="73"/>
+      <c r="F24" s="73"/>
       <c r="G24" s="35" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="H24" s="35" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="I24" s="41" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J24" s="38"/>
       <c r="K24" s="38"/>
     </row>
     <row r="25" spans="1:11" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A25" s="41" t="s">
-        <v>147</v>
-      </c>
-      <c r="B25" s="80"/>
-      <c r="C25" s="80"/>
+        <v>146</v>
+      </c>
+      <c r="B25" s="69"/>
+      <c r="C25" s="69"/>
       <c r="D25" s="40" t="s">
-        <v>231</v>
-      </c>
-      <c r="E25" s="83"/>
-      <c r="F25" s="83"/>
+        <v>230</v>
+      </c>
+      <c r="E25" s="73"/>
+      <c r="F25" s="73"/>
       <c r="G25" s="35" t="s">
-        <v>193</v>
-      </c>
-      <c r="H25" s="78" t="s">
-        <v>239</v>
+        <v>192</v>
+      </c>
+      <c r="H25" s="67" t="s">
+        <v>238</v>
       </c>
       <c r="I25" s="41" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J25" s="38"/>
       <c r="K25" s="38"/>
     </row>
     <row r="26" spans="1:11" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A26" s="41" t="s">
-        <v>148</v>
-      </c>
-      <c r="B26" s="80"/>
-      <c r="C26" s="80"/>
+        <v>147</v>
+      </c>
+      <c r="B26" s="69"/>
+      <c r="C26" s="69"/>
       <c r="D26" s="40" t="s">
-        <v>233</v>
-      </c>
-      <c r="E26" s="83"/>
-      <c r="F26" s="83"/>
+        <v>232</v>
+      </c>
+      <c r="E26" s="73"/>
+      <c r="F26" s="73"/>
       <c r="G26" s="35" t="s">
-        <v>235</v>
-      </c>
-      <c r="H26" s="79"/>
+        <v>234</v>
+      </c>
+      <c r="H26" s="68"/>
       <c r="I26" s="41" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J26" s="38"/>
       <c r="K26" s="38"/>
     </row>
     <row r="27" spans="1:11" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A27" s="41" t="s">
-        <v>149</v>
-      </c>
-      <c r="B27" s="80"/>
-      <c r="C27" s="79"/>
+        <v>148</v>
+      </c>
+      <c r="B27" s="69"/>
+      <c r="C27" s="68"/>
       <c r="D27" s="40" t="s">
-        <v>232</v>
-      </c>
-      <c r="E27" s="83"/>
-      <c r="F27" s="77"/>
+        <v>231</v>
+      </c>
+      <c r="E27" s="73"/>
+      <c r="F27" s="74"/>
       <c r="G27" s="35" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="H27" s="35" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="I27" s="41" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J27" s="38"/>
       <c r="K27" s="38"/>
     </row>
     <row r="28" spans="1:11" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A28" s="41" t="s">
-        <v>150</v>
-      </c>
-      <c r="B28" s="80"/>
-      <c r="C28" s="78" t="s">
-        <v>198</v>
+        <v>149</v>
+      </c>
+      <c r="B28" s="69"/>
+      <c r="C28" s="67" t="s">
+        <v>197</v>
       </c>
       <c r="D28" s="35" t="s">
-        <v>166</v>
-      </c>
-      <c r="E28" s="83"/>
+        <v>165</v>
+      </c>
+      <c r="E28" s="73"/>
       <c r="F28" s="37" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="G28" s="36" t="s">
+        <v>193</v>
+      </c>
+      <c r="H28" s="35" t="s">
         <v>194</v>
       </c>
-      <c r="H28" s="35" t="s">
-        <v>195</v>
-      </c>
       <c r="I28" s="41" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J28" s="38"/>
       <c r="K28" s="38"/>
     </row>
     <row r="29" spans="1:11" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A29" s="41" t="s">
-        <v>151</v>
-      </c>
-      <c r="B29" s="80"/>
-      <c r="C29" s="80"/>
+        <v>150</v>
+      </c>
+      <c r="B29" s="69"/>
+      <c r="C29" s="69"/>
       <c r="D29" s="36" t="s">
+        <v>201</v>
+      </c>
+      <c r="E29" s="73"/>
+      <c r="F29" s="72" t="s">
+        <v>195</v>
+      </c>
+      <c r="G29" s="35" t="s">
         <v>202</v>
       </c>
-      <c r="E29" s="83"/>
-      <c r="F29" s="76" t="s">
-        <v>196</v>
-      </c>
-      <c r="G29" s="35" t="s">
-        <v>203</v>
-      </c>
       <c r="H29" s="35" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="I29" s="41" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J29" s="38"/>
       <c r="K29" s="38"/>
     </row>
     <row r="30" spans="1:11" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A30" s="41" t="s">
-        <v>152</v>
-      </c>
-      <c r="B30" s="80"/>
-      <c r="C30" s="80"/>
+        <v>151</v>
+      </c>
+      <c r="B30" s="69"/>
+      <c r="C30" s="69"/>
       <c r="D30" s="38" t="s">
+        <v>203</v>
+      </c>
+      <c r="E30" s="73"/>
+      <c r="F30" s="74"/>
+      <c r="G30" s="35" t="s">
         <v>204</v>
       </c>
-      <c r="E30" s="83"/>
-      <c r="F30" s="77"/>
-      <c r="G30" s="35" t="s">
+      <c r="H30" s="38" t="s">
         <v>205</v>
       </c>
-      <c r="H30" s="38" t="s">
-        <v>206</v>
-      </c>
       <c r="I30" s="41" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J30" s="38"/>
       <c r="K30" s="38"/>
     </row>
     <row r="31" spans="1:11" ht="94.5" x14ac:dyDescent="0.25">
       <c r="A31" s="41" t="s">
-        <v>153</v>
-      </c>
-      <c r="B31" s="80"/>
-      <c r="C31" s="79"/>
+        <v>152</v>
+      </c>
+      <c r="B31" s="69"/>
+      <c r="C31" s="68"/>
       <c r="D31" s="35" t="s">
+        <v>207</v>
+      </c>
+      <c r="E31" s="74"/>
+      <c r="F31" s="37" t="s">
         <v>208</v>
       </c>
-      <c r="E31" s="77"/>
-      <c r="F31" s="37" t="s">
-        <v>209</v>
-      </c>
       <c r="G31" s="35" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="H31" s="44" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="I31" s="41" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J31" s="38"/>
       <c r="K31" s="38"/>
     </row>
     <row r="32" spans="1:11" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A32" s="41" t="s">
-        <v>154</v>
-      </c>
-      <c r="B32" s="80"/>
-      <c r="C32" s="78" t="s">
-        <v>207</v>
+        <v>153</v>
+      </c>
+      <c r="B32" s="69"/>
+      <c r="C32" s="67" t="s">
+        <v>206</v>
       </c>
       <c r="D32" s="35" t="s">
+        <v>165</v>
+      </c>
+      <c r="E32" s="72" t="s">
         <v>166</v>
       </c>
-      <c r="E32" s="76" t="s">
-        <v>167</v>
-      </c>
       <c r="F32" s="37" t="s">
+        <v>209</v>
+      </c>
+      <c r="G32" s="38" t="s">
         <v>210</v>
       </c>
-      <c r="G32" s="38" t="s">
+      <c r="H32" s="35" t="s">
         <v>211</v>
       </c>
-      <c r="H32" s="35" t="s">
-        <v>212</v>
-      </c>
       <c r="I32" s="41" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J32" s="38"/>
       <c r="K32" s="38"/>
     </row>
     <row r="33" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="41" t="s">
-        <v>255</v>
-      </c>
-      <c r="B33" s="80"/>
-      <c r="C33" s="80"/>
+        <v>252</v>
+      </c>
+      <c r="B33" s="69"/>
+      <c r="C33" s="69"/>
       <c r="D33" s="20" t="s">
-        <v>213</v>
-      </c>
-      <c r="E33" s="83"/>
-      <c r="F33" s="87" t="s">
+        <v>212</v>
+      </c>
+      <c r="E33" s="73"/>
+      <c r="F33" s="70" t="s">
+        <v>215</v>
+      </c>
+      <c r="G33" s="20" t="s">
+        <v>55</v>
+      </c>
+      <c r="H33" s="65" t="s">
         <v>216</v>
       </c>
-      <c r="G33" s="20" t="s">
-        <v>56</v>
-      </c>
-      <c r="H33" s="64" t="s">
-        <v>217</v>
-      </c>
       <c r="I33" s="39" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J33" s="20"/>
       <c r="K33" s="20"/>
     </row>
     <row r="34" spans="1:11" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A34" s="41" t="s">
-        <v>256</v>
-      </c>
-      <c r="B34" s="80"/>
-      <c r="C34" s="80"/>
+        <v>253</v>
+      </c>
+      <c r="B34" s="69"/>
+      <c r="C34" s="69"/>
       <c r="D34" s="40" t="s">
-        <v>214</v>
-      </c>
-      <c r="E34" s="83"/>
-      <c r="F34" s="89"/>
+        <v>213</v>
+      </c>
+      <c r="E34" s="73"/>
+      <c r="F34" s="75"/>
       <c r="G34" s="20" t="s">
-        <v>66</v>
-      </c>
-      <c r="H34" s="64"/>
+        <v>65</v>
+      </c>
+      <c r="H34" s="65"/>
       <c r="I34" s="39" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J34" s="20"/>
       <c r="K34" s="20"/>
     </row>
     <row r="35" spans="1:11" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A35" s="41" t="s">
-        <v>257</v>
-      </c>
-      <c r="B35" s="80"/>
-      <c r="C35" s="80"/>
+        <v>254</v>
+      </c>
+      <c r="B35" s="69"/>
+      <c r="C35" s="69"/>
       <c r="D35" s="40" t="s">
-        <v>58</v>
-      </c>
-      <c r="E35" s="83"/>
-      <c r="F35" s="89"/>
+        <v>57</v>
+      </c>
+      <c r="E35" s="73"/>
+      <c r="F35" s="75"/>
       <c r="G35" s="20" t="s">
+        <v>59</v>
+      </c>
+      <c r="H35" s="65" t="s">
         <v>60</v>
       </c>
-      <c r="H35" s="64" t="s">
-        <v>61</v>
-      </c>
       <c r="I35" s="39" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J35" s="20"/>
       <c r="K35" s="20"/>
     </row>
     <row r="36" spans="1:11" ht="56.25" x14ac:dyDescent="0.25">
       <c r="A36" s="41" t="s">
-        <v>155</v>
-      </c>
-      <c r="B36" s="80"/>
-      <c r="C36" s="80"/>
+        <v>154</v>
+      </c>
+      <c r="B36" s="69"/>
+      <c r="C36" s="69"/>
       <c r="D36" s="40" t="s">
-        <v>215</v>
-      </c>
-      <c r="E36" s="83"/>
-      <c r="F36" s="88"/>
+        <v>214</v>
+      </c>
+      <c r="E36" s="73"/>
+      <c r="F36" s="71"/>
       <c r="G36" s="20" t="s">
-        <v>62</v>
-      </c>
-      <c r="H36" s="64"/>
+        <v>61</v>
+      </c>
+      <c r="H36" s="65"/>
       <c r="I36" s="39" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J36" s="20"/>
       <c r="K36" s="20"/>
     </row>
     <row r="37" spans="1:11" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A37" s="41" t="s">
-        <v>258</v>
-      </c>
-      <c r="B37" s="80"/>
-      <c r="C37" s="80"/>
+        <v>255</v>
+      </c>
+      <c r="B37" s="69"/>
+      <c r="C37" s="69"/>
       <c r="D37" s="35" t="s">
-        <v>168</v>
-      </c>
-      <c r="E37" s="83"/>
+        <v>167</v>
+      </c>
+      <c r="E37" s="73"/>
       <c r="F37" s="43" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="G37" s="35" t="s">
+        <v>217</v>
+      </c>
+      <c r="H37" s="35" t="s">
         <v>218</v>
       </c>
-      <c r="H37" s="35" t="s">
-        <v>219</v>
-      </c>
       <c r="I37" s="41" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J37" s="38"/>
       <c r="K37" s="38"/>
     </row>
     <row r="38" spans="1:11" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A38" s="41" t="s">
-        <v>156</v>
-      </c>
-      <c r="B38" s="80"/>
-      <c r="C38" s="80"/>
+        <v>155</v>
+      </c>
+      <c r="B38" s="69"/>
+      <c r="C38" s="69"/>
       <c r="D38" s="38" t="s">
+        <v>220</v>
+      </c>
+      <c r="E38" s="73"/>
+      <c r="F38" s="67" t="s">
+        <v>219</v>
+      </c>
+      <c r="G38" s="35" t="s">
         <v>221</v>
       </c>
-      <c r="E38" s="83"/>
-      <c r="F38" s="78" t="s">
-        <v>220</v>
-      </c>
-      <c r="G38" s="35" t="s">
+      <c r="H38" s="35" t="s">
         <v>222</v>
       </c>
-      <c r="H38" s="35" t="s">
-        <v>223</v>
-      </c>
       <c r="I38" s="41" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J38" s="38"/>
       <c r="K38" s="38"/>
     </row>
     <row r="39" spans="1:11" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A39" s="41" t="s">
-        <v>157</v>
-      </c>
-      <c r="B39" s="80"/>
-      <c r="C39" s="80"/>
+        <v>156</v>
+      </c>
+      <c r="B39" s="69"/>
+      <c r="C39" s="69"/>
       <c r="D39" s="38" t="s">
-        <v>227</v>
-      </c>
-      <c r="E39" s="83"/>
-      <c r="F39" s="80"/>
+        <v>226</v>
+      </c>
+      <c r="E39" s="73"/>
+      <c r="F39" s="69"/>
       <c r="G39" s="35" t="s">
+        <v>224</v>
+      </c>
+      <c r="H39" s="36" t="s">
         <v>225</v>
       </c>
-      <c r="H39" s="36" t="s">
-        <v>226</v>
-      </c>
       <c r="I39" s="41" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="J39" s="38"/>
       <c r="K39" s="38"/>
     </row>
     <row r="40" spans="1:11" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A40" s="41" t="s">
-        <v>158</v>
-      </c>
-      <c r="B40" s="79"/>
-      <c r="C40" s="79"/>
+        <v>157</v>
+      </c>
+      <c r="B40" s="68"/>
+      <c r="C40" s="68"/>
       <c r="D40" s="38" t="s">
-        <v>224</v>
-      </c>
-      <c r="E40" s="77"/>
-      <c r="F40" s="79"/>
+        <v>223</v>
+      </c>
+      <c r="E40" s="74"/>
+      <c r="F40" s="68"/>
       <c r="G40" s="35" t="s">
+        <v>227</v>
+      </c>
+      <c r="H40" s="36" t="s">
         <v>228</v>
       </c>
-      <c r="H40" s="36" t="s">
-        <v>229</v>
-      </c>
       <c r="I40" s="41" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="J40" s="38"/>
       <c r="K40" s="38"/>
     </row>
     <row r="41" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A41" s="41" t="s">
-        <v>259</v>
-      </c>
-      <c r="B41" s="78" t="s">
-        <v>86</v>
-      </c>
-      <c r="C41" s="65" t="s">
-        <v>106</v>
+        <v>256</v>
+      </c>
+      <c r="B41" s="67" t="s">
+        <v>85</v>
+      </c>
+      <c r="C41" s="64" t="s">
+        <v>105</v>
       </c>
       <c r="D41" s="20" t="s">
-        <v>96</v>
-      </c>
-      <c r="E41" s="87" t="s">
-        <v>167</v>
+        <v>95</v>
+      </c>
+      <c r="E41" s="70" t="s">
+        <v>166</v>
       </c>
       <c r="F41" s="21" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="G41" s="20"/>
       <c r="H41" s="40" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="I41" s="39" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J41" s="38"/>
       <c r="K41" s="38"/>
     </row>
     <row r="42" spans="1:11" ht="56.25" x14ac:dyDescent="0.3">
       <c r="A42" s="41" t="s">
-        <v>159</v>
-      </c>
-      <c r="B42" s="79"/>
-      <c r="C42" s="65"/>
+        <v>158</v>
+      </c>
+      <c r="B42" s="68"/>
+      <c r="C42" s="64"/>
       <c r="D42" s="20" t="s">
-        <v>97</v>
-      </c>
-      <c r="E42" s="88"/>
+        <v>96</v>
+      </c>
+      <c r="E42" s="71"/>
       <c r="F42" s="21" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="G42" s="25"/>
       <c r="H42" s="40" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="I42" s="39" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J42" s="38"/>
       <c r="K42" s="38"/>
     </row>
   </sheetData>
   <mergeCells count="29">
+    <mergeCell ref="E17:E18"/>
+    <mergeCell ref="C17:C18"/>
+    <mergeCell ref="F15:F16"/>
+    <mergeCell ref="C14:C16"/>
+    <mergeCell ref="B9:B13"/>
+    <mergeCell ref="E9:E13"/>
+    <mergeCell ref="E14:E16"/>
+    <mergeCell ref="F29:F30"/>
+    <mergeCell ref="E22:E31"/>
+    <mergeCell ref="C28:C31"/>
+    <mergeCell ref="C19:C21"/>
+    <mergeCell ref="E19:E21"/>
+    <mergeCell ref="F20:F21"/>
     <mergeCell ref="B41:B42"/>
     <mergeCell ref="B1:E1"/>
     <mergeCell ref="B2:E2"/>
@@ -3967,40 +4055,27 @@
     <mergeCell ref="H33:H34"/>
     <mergeCell ref="H35:H36"/>
     <mergeCell ref="F33:F36"/>
-    <mergeCell ref="F29:F30"/>
-    <mergeCell ref="E22:E31"/>
-    <mergeCell ref="C28:C31"/>
-    <mergeCell ref="C19:C21"/>
-    <mergeCell ref="E19:E21"/>
-    <mergeCell ref="F20:F21"/>
-    <mergeCell ref="E17:E18"/>
-    <mergeCell ref="C17:C18"/>
-    <mergeCell ref="F15:F16"/>
-    <mergeCell ref="C14:C16"/>
-    <mergeCell ref="B9:B13"/>
-    <mergeCell ref="E9:E13"/>
-    <mergeCell ref="E14:E16"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="I8:I32 I37:I42">
-    <cfRule type="containsText" dxfId="5" priority="7" operator="containsText" text="Untested">
+    <cfRule type="containsText" dxfId="8" priority="7" operator="containsText" text="Untested">
       <formula>NOT(ISERROR(SEARCH("Untested",I8)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="4" priority="8" operator="containsText" text="Passed">
+    <cfRule type="containsText" dxfId="7" priority="8" operator="containsText" text="Passed">
       <formula>NOT(ISERROR(SEARCH("Passed",I8)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="3" priority="9" operator="containsText" text="Failed">
+    <cfRule type="containsText" dxfId="6" priority="9" operator="containsText" text="Failed">
       <formula>NOT(ISERROR(SEARCH("Failed",I8)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I33:I36">
-    <cfRule type="containsText" dxfId="2" priority="4" operator="containsText" text="Untested">
+    <cfRule type="containsText" dxfId="5" priority="4" operator="containsText" text="Untested">
       <formula>NOT(ISERROR(SEARCH("Untested",I33)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="1" priority="5" operator="containsText" text="Passed">
+    <cfRule type="containsText" dxfId="4" priority="5" operator="containsText" text="Passed">
       <formula>NOT(ISERROR(SEARCH("Passed",I33)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="0" priority="6" operator="containsText" text="Failed">
+    <cfRule type="containsText" dxfId="3" priority="6" operator="containsText" text="Failed">
       <formula>NOT(ISERROR(SEARCH("Failed",I33)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4012,4 +4087,608 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C9B0476B-3B06-4146-9968-E5376D04BD7B}">
+  <dimension ref="A1:K30"/>
+  <sheetViews>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="7" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C10" sqref="C10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.42578125" style="86" customWidth="1"/>
+    <col min="2" max="2" width="25.5703125" style="90" customWidth="1"/>
+    <col min="3" max="3" width="27.85546875" style="91" customWidth="1"/>
+    <col min="4" max="4" width="26.7109375" style="90" customWidth="1"/>
+    <col min="5" max="5" width="28.28515625" style="84" customWidth="1"/>
+    <col min="6" max="6" width="32.7109375" style="84" customWidth="1"/>
+    <col min="7" max="7" width="26.85546875" style="84" customWidth="1"/>
+    <col min="8" max="8" width="24.140625" style="84" customWidth="1"/>
+    <col min="9" max="9" width="23.5703125" style="85" customWidth="1"/>
+    <col min="10" max="10" width="18.140625" style="84" customWidth="1"/>
+    <col min="11" max="11" width="12.28515625" style="84" customWidth="1"/>
+    <col min="12" max="16384" width="9.140625" style="84"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="83" t="s">
+        <v>122</v>
+      </c>
+      <c r="B1" s="81" t="s">
+        <v>286</v>
+      </c>
+      <c r="C1" s="81"/>
+      <c r="D1" s="81"/>
+      <c r="E1" s="81"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="3"/>
+      <c r="J1" s="1"/>
+      <c r="K1" s="1"/>
+    </row>
+    <row r="2" spans="1:11" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A2" s="83" t="s">
+        <v>123</v>
+      </c>
+      <c r="B2" s="77"/>
+      <c r="C2" s="77"/>
+      <c r="D2" s="77"/>
+      <c r="E2" s="77"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="3"/>
+      <c r="J2" s="1"/>
+      <c r="K2" s="1"/>
+    </row>
+    <row r="3" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="83" t="s">
+        <v>124</v>
+      </c>
+      <c r="B3" s="82" t="s">
+        <v>129</v>
+      </c>
+      <c r="C3" s="82"/>
+      <c r="D3" s="82"/>
+      <c r="E3" s="82"/>
+      <c r="F3" s="4"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="3"/>
+      <c r="J3" s="1"/>
+      <c r="K3" s="1"/>
+    </row>
+    <row r="4" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="83" t="s">
+        <v>125</v>
+      </c>
+      <c r="B4" s="50" t="s">
+        <v>126</v>
+      </c>
+      <c r="C4" s="51" t="s">
+        <v>97</v>
+      </c>
+      <c r="D4" s="50" t="s">
+        <v>127</v>
+      </c>
+      <c r="E4" s="30" t="s">
+        <v>109</v>
+      </c>
+      <c r="F4" s="4"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+      <c r="I4" s="3"/>
+      <c r="J4" s="1"/>
+      <c r="K4" s="1"/>
+    </row>
+    <row r="5" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="50">
+        <f>COUNTA(I8:I42)</f>
+        <v>20</v>
+      </c>
+      <c r="B5" s="50">
+        <f>COUNTIF(I8:I42,I8)</f>
+        <v>20</v>
+      </c>
+      <c r="C5" s="51">
+        <f>COUNTIF(I8:I42,"Failed")</f>
+        <v>0</v>
+      </c>
+      <c r="D5" s="50">
+        <f>COUNTIF(I8:I42,"Untested")</f>
+        <v>0</v>
+      </c>
+      <c r="E5" s="30">
+        <f>COUNTIF(I8:I42,"N/A")</f>
+        <v>0</v>
+      </c>
+      <c r="F5" s="4"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="3"/>
+      <c r="J5" s="1"/>
+      <c r="K5" s="1"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" s="85"/>
+      <c r="C6" s="94"/>
+    </row>
+    <row r="7" spans="1:11" s="86" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="33" t="s">
+        <v>0</v>
+      </c>
+      <c r="B7" s="34" t="s">
+        <v>1</v>
+      </c>
+      <c r="C7" s="88" t="s">
+        <v>2</v>
+      </c>
+      <c r="D7" s="34" t="s">
+        <v>3</v>
+      </c>
+      <c r="E7" s="33" t="s">
+        <v>4</v>
+      </c>
+      <c r="F7" s="33" t="s">
+        <v>5</v>
+      </c>
+      <c r="G7" s="33" t="s">
+        <v>6</v>
+      </c>
+      <c r="H7" s="33" t="s">
+        <v>7</v>
+      </c>
+      <c r="I7" s="34" t="s">
+        <v>8</v>
+      </c>
+      <c r="J7" s="33" t="s">
+        <v>6</v>
+      </c>
+      <c r="K7" s="33" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="90" x14ac:dyDescent="0.25">
+      <c r="A8" s="87" t="s">
+        <v>263</v>
+      </c>
+      <c r="B8" s="93" t="s">
+        <v>29</v>
+      </c>
+      <c r="C8" s="95" t="s">
+        <v>287</v>
+      </c>
+      <c r="D8" s="93" t="s">
+        <v>288</v>
+      </c>
+      <c r="E8" s="89" t="s">
+        <v>290</v>
+      </c>
+      <c r="F8" s="89" t="s">
+        <v>291</v>
+      </c>
+      <c r="G8" s="89" t="s">
+        <v>294</v>
+      </c>
+      <c r="H8" s="89" t="s">
+        <v>295</v>
+      </c>
+      <c r="I8" s="50" t="s">
+        <v>35</v>
+      </c>
+      <c r="J8" s="89"/>
+      <c r="K8" s="89"/>
+    </row>
+    <row r="9" spans="1:11" ht="105" x14ac:dyDescent="0.25">
+      <c r="A9" s="87" t="s">
+        <v>264</v>
+      </c>
+      <c r="B9" s="93"/>
+      <c r="C9" s="96"/>
+      <c r="D9" s="93" t="s">
+        <v>289</v>
+      </c>
+      <c r="E9" s="89" t="s">
+        <v>292</v>
+      </c>
+      <c r="F9" s="89" t="s">
+        <v>297</v>
+      </c>
+      <c r="G9" s="89" t="s">
+        <v>293</v>
+      </c>
+      <c r="H9" s="89" t="s">
+        <v>296</v>
+      </c>
+      <c r="I9" s="50" t="s">
+        <v>35</v>
+      </c>
+      <c r="J9" s="89"/>
+      <c r="K9" s="89"/>
+    </row>
+    <row r="10" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A10" s="87" t="s">
+        <v>265</v>
+      </c>
+      <c r="B10" s="93"/>
+      <c r="C10" s="89" t="s">
+        <v>298</v>
+      </c>
+      <c r="D10" s="93"/>
+      <c r="E10" s="89"/>
+      <c r="F10" s="89"/>
+      <c r="G10" s="89"/>
+      <c r="H10" s="89"/>
+      <c r="I10" s="50" t="s">
+        <v>35</v>
+      </c>
+      <c r="J10" s="89"/>
+      <c r="K10" s="89"/>
+    </row>
+    <row r="11" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A11" s="87" t="s">
+        <v>266</v>
+      </c>
+      <c r="B11" s="93"/>
+      <c r="C11" s="89"/>
+      <c r="D11" s="93"/>
+      <c r="E11" s="89"/>
+      <c r="F11" s="89"/>
+      <c r="G11" s="89"/>
+      <c r="H11" s="89"/>
+      <c r="I11" s="50" t="s">
+        <v>35</v>
+      </c>
+      <c r="J11" s="89"/>
+      <c r="K11" s="89"/>
+    </row>
+    <row r="12" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A12" s="87" t="s">
+        <v>267</v>
+      </c>
+      <c r="B12" s="93"/>
+      <c r="C12" s="89"/>
+      <c r="D12" s="93"/>
+      <c r="E12" s="89"/>
+      <c r="F12" s="89"/>
+      <c r="G12" s="89"/>
+      <c r="H12" s="89"/>
+      <c r="I12" s="50" t="s">
+        <v>35</v>
+      </c>
+      <c r="J12" s="89"/>
+      <c r="K12" s="89"/>
+    </row>
+    <row r="13" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A13" s="87" t="s">
+        <v>268</v>
+      </c>
+      <c r="B13" s="93"/>
+      <c r="C13" s="89"/>
+      <c r="D13" s="93"/>
+      <c r="E13" s="89"/>
+      <c r="F13" s="89"/>
+      <c r="G13" s="89"/>
+      <c r="H13" s="89"/>
+      <c r="I13" s="50" t="s">
+        <v>35</v>
+      </c>
+      <c r="J13" s="89"/>
+      <c r="K13" s="89"/>
+    </row>
+    <row r="14" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A14" s="87" t="s">
+        <v>269</v>
+      </c>
+      <c r="B14" s="93"/>
+      <c r="C14" s="89"/>
+      <c r="D14" s="93"/>
+      <c r="E14" s="89"/>
+      <c r="F14" s="89"/>
+      <c r="G14" s="89"/>
+      <c r="H14" s="89"/>
+      <c r="I14" s="50" t="s">
+        <v>35</v>
+      </c>
+      <c r="J14" s="89"/>
+      <c r="K14" s="89"/>
+    </row>
+    <row r="15" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A15" s="87" t="s">
+        <v>270</v>
+      </c>
+      <c r="B15" s="93"/>
+      <c r="C15" s="89"/>
+      <c r="D15" s="93"/>
+      <c r="E15" s="89"/>
+      <c r="F15" s="89"/>
+      <c r="G15" s="89"/>
+      <c r="H15" s="89"/>
+      <c r="I15" s="50" t="s">
+        <v>35</v>
+      </c>
+      <c r="J15" s="89"/>
+      <c r="K15" s="89"/>
+    </row>
+    <row r="16" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A16" s="87" t="s">
+        <v>271</v>
+      </c>
+      <c r="B16" s="93"/>
+      <c r="C16" s="89"/>
+      <c r="D16" s="93"/>
+      <c r="E16" s="89"/>
+      <c r="F16" s="89"/>
+      <c r="G16" s="89"/>
+      <c r="H16" s="89"/>
+      <c r="I16" s="50" t="s">
+        <v>35</v>
+      </c>
+      <c r="J16" s="89"/>
+      <c r="K16" s="89"/>
+    </row>
+    <row r="17" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A17" s="87" t="s">
+        <v>272</v>
+      </c>
+      <c r="B17" s="93"/>
+      <c r="C17" s="89"/>
+      <c r="D17" s="93"/>
+      <c r="E17" s="89"/>
+      <c r="F17" s="89"/>
+      <c r="G17" s="89"/>
+      <c r="H17" s="89"/>
+      <c r="I17" s="50" t="s">
+        <v>35</v>
+      </c>
+      <c r="J17" s="89"/>
+      <c r="K17" s="89"/>
+    </row>
+    <row r="18" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A18" s="87" t="s">
+        <v>273</v>
+      </c>
+      <c r="B18" s="93"/>
+      <c r="C18" s="89"/>
+      <c r="D18" s="93"/>
+      <c r="E18" s="89"/>
+      <c r="F18" s="89"/>
+      <c r="G18" s="89"/>
+      <c r="H18" s="89"/>
+      <c r="I18" s="50" t="s">
+        <v>35</v>
+      </c>
+      <c r="J18" s="89"/>
+      <c r="K18" s="89"/>
+    </row>
+    <row r="19" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A19" s="87" t="s">
+        <v>274</v>
+      </c>
+      <c r="B19" s="93"/>
+      <c r="C19" s="89"/>
+      <c r="D19" s="93"/>
+      <c r="E19" s="89"/>
+      <c r="F19" s="89"/>
+      <c r="G19" s="89"/>
+      <c r="H19" s="89"/>
+      <c r="I19" s="50" t="s">
+        <v>35</v>
+      </c>
+      <c r="J19" s="89"/>
+      <c r="K19" s="89"/>
+    </row>
+    <row r="20" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A20" s="87" t="s">
+        <v>275</v>
+      </c>
+      <c r="B20" s="93"/>
+      <c r="C20" s="89"/>
+      <c r="D20" s="93"/>
+      <c r="E20" s="89"/>
+      <c r="F20" s="89"/>
+      <c r="G20" s="89"/>
+      <c r="H20" s="89"/>
+      <c r="I20" s="50" t="s">
+        <v>35</v>
+      </c>
+      <c r="J20" s="89"/>
+      <c r="K20" s="89"/>
+    </row>
+    <row r="21" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A21" s="87" t="s">
+        <v>276</v>
+      </c>
+      <c r="B21" s="93"/>
+      <c r="C21" s="89"/>
+      <c r="D21" s="93"/>
+      <c r="E21" s="89"/>
+      <c r="F21" s="89"/>
+      <c r="G21" s="89"/>
+      <c r="H21" s="89"/>
+      <c r="I21" s="50" t="s">
+        <v>35</v>
+      </c>
+      <c r="J21" s="89"/>
+      <c r="K21" s="89"/>
+    </row>
+    <row r="22" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A22" s="87" t="s">
+        <v>277</v>
+      </c>
+      <c r="B22" s="93"/>
+      <c r="C22" s="89"/>
+      <c r="D22" s="93"/>
+      <c r="E22" s="89"/>
+      <c r="F22" s="89"/>
+      <c r="G22" s="89"/>
+      <c r="H22" s="89"/>
+      <c r="I22" s="50" t="s">
+        <v>35</v>
+      </c>
+      <c r="J22" s="89"/>
+      <c r="K22" s="89"/>
+    </row>
+    <row r="23" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A23" s="87" t="s">
+        <v>278</v>
+      </c>
+      <c r="B23" s="93"/>
+      <c r="C23" s="89"/>
+      <c r="D23" s="93"/>
+      <c r="E23" s="89"/>
+      <c r="F23" s="89"/>
+      <c r="G23" s="89"/>
+      <c r="H23" s="89"/>
+      <c r="I23" s="50" t="s">
+        <v>35</v>
+      </c>
+      <c r="J23" s="89"/>
+      <c r="K23" s="89"/>
+    </row>
+    <row r="24" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A24" s="87" t="s">
+        <v>279</v>
+      </c>
+      <c r="B24" s="93"/>
+      <c r="C24" s="89"/>
+      <c r="D24" s="93"/>
+      <c r="E24" s="89"/>
+      <c r="F24" s="89"/>
+      <c r="G24" s="89"/>
+      <c r="H24" s="89"/>
+      <c r="I24" s="50" t="s">
+        <v>35</v>
+      </c>
+      <c r="J24" s="89"/>
+      <c r="K24" s="89"/>
+    </row>
+    <row r="25" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A25" s="87" t="s">
+        <v>280</v>
+      </c>
+      <c r="B25" s="93"/>
+      <c r="C25" s="89"/>
+      <c r="D25" s="93"/>
+      <c r="E25" s="89"/>
+      <c r="F25" s="89"/>
+      <c r="G25" s="89"/>
+      <c r="H25" s="89"/>
+      <c r="I25" s="50" t="s">
+        <v>35</v>
+      </c>
+      <c r="J25" s="89"/>
+      <c r="K25" s="89"/>
+    </row>
+    <row r="26" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A26" s="87" t="s">
+        <v>281</v>
+      </c>
+      <c r="B26" s="93"/>
+      <c r="C26" s="89"/>
+      <c r="D26" s="93"/>
+      <c r="E26" s="89"/>
+      <c r="F26" s="89"/>
+      <c r="G26" s="89"/>
+      <c r="H26" s="89"/>
+      <c r="I26" s="50" t="s">
+        <v>35</v>
+      </c>
+      <c r="J26" s="89"/>
+      <c r="K26" s="89"/>
+    </row>
+    <row r="27" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A27" s="87" t="s">
+        <v>282</v>
+      </c>
+      <c r="B27" s="93"/>
+      <c r="C27" s="89"/>
+      <c r="D27" s="93"/>
+      <c r="E27" s="89"/>
+      <c r="F27" s="89"/>
+      <c r="G27" s="89"/>
+      <c r="H27" s="89"/>
+      <c r="I27" s="50" t="s">
+        <v>35</v>
+      </c>
+      <c r="J27" s="89"/>
+      <c r="K27" s="89"/>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A28" s="87" t="s">
+        <v>283</v>
+      </c>
+      <c r="B28" s="93"/>
+      <c r="C28" s="89"/>
+      <c r="D28" s="93"/>
+      <c r="E28" s="89"/>
+      <c r="F28" s="89"/>
+      <c r="G28" s="89"/>
+      <c r="H28" s="89"/>
+      <c r="I28" s="92"/>
+      <c r="J28" s="89"/>
+      <c r="K28" s="89"/>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A29" s="87" t="s">
+        <v>284</v>
+      </c>
+      <c r="B29" s="93"/>
+      <c r="C29" s="89"/>
+      <c r="D29" s="93"/>
+      <c r="E29" s="89"/>
+      <c r="F29" s="89"/>
+      <c r="G29" s="89"/>
+      <c r="H29" s="89"/>
+      <c r="I29" s="92"/>
+      <c r="J29" s="89"/>
+      <c r="K29" s="89"/>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A30" s="87" t="s">
+        <v>285</v>
+      </c>
+      <c r="B30" s="93"/>
+      <c r="C30" s="89"/>
+      <c r="D30" s="93"/>
+      <c r="E30" s="89"/>
+      <c r="F30" s="89"/>
+      <c r="G30" s="89"/>
+      <c r="H30" s="89"/>
+      <c r="I30" s="92"/>
+      <c r="J30" s="89"/>
+      <c r="K30" s="89"/>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="B1:E1"/>
+    <mergeCell ref="B2:E2"/>
+    <mergeCell ref="B3:E3"/>
+  </mergeCells>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <conditionalFormatting sqref="I8:I27">
+    <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="Untested">
+      <formula>NOT(ISERROR(SEARCH("Untested",I8)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="Passed">
+      <formula>NOT(ISERROR(SEARCH("Passed",I8)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="0" priority="3" operator="containsText" text="Failed">
+      <formula>NOT(ISERROR(SEARCH("Failed",I8)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I7:I27" xr:uid="{E4E2C4F3-03D6-47C3-B651-D6C1663F6D32}">
+      <formula1>"Passed, Failed, Untested, N/A"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>